<commit_message>
Support for cancelled actions
Add new column in excel sheet
</commit_message>
<xml_diff>
--- a/data/Registro_acciones.xlsx
+++ b/data/Registro_acciones.xlsx
@@ -22,32 +22,8 @@
 </workbook>
 </file>
 
-<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
-  <authors>
-    <author> </author>
-  </authors>
-  <commentList>
-    <comment ref="D2" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="0"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">Si, si, Sí, sí, SÍ, SI, s o S para determinarla como zona de actuación finalizada</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="34">
   <si>
     <t xml:space="preserve">ACCIONES DE VOLUNTARIADO</t>
   </si>
@@ -61,7 +37,7 @@
     <t xml:space="preserve">LUGAR</t>
   </si>
   <si>
-    <t xml:space="preserve">ULTIMA</t>
+    <t xml:space="preserve">Notas</t>
   </si>
   <si>
     <t xml:space="preserve">Dificultad</t>
@@ -107,6 +83,9 @@
   </si>
   <si>
     <t xml:space="preserve">Baja/media/alta</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CANCELADA</t>
   </si>
   <si>
     <t xml:space="preserve">CANCELADA por prevención COVID19</t>
@@ -445,7 +424,7 @@
       <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4609375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.48046875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="4.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="10.86"/>
@@ -972,9 +951,11 @@
       <c r="C33" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="D33" s="14"/>
+      <c r="D33" s="14" t="s">
+        <v>20</v>
+      </c>
       <c r="E33" s="15" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F33" s="16"/>
       <c r="G33" s="15"/>
@@ -1011,7 +992,7 @@
       </c>
       <c r="D34" s="9"/>
       <c r="E34" s="17" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F34" s="10"/>
       <c r="G34" s="17"/>
@@ -1048,7 +1029,7 @@
       </c>
       <c r="D35" s="9"/>
       <c r="E35" s="11" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F35" s="10"/>
       <c r="H35" s="11"/>
@@ -1080,11 +1061,11 @@
         <v>43993</v>
       </c>
       <c r="C37" s="9" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D37" s="9"/>
       <c r="E37" s="11" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F37" s="10"/>
       <c r="G37" s="11"/>
@@ -1102,7 +1083,7 @@
       </c>
       <c r="D38" s="9"/>
       <c r="E38" s="11" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F38" s="10"/>
       <c r="H38" s="11"/>
@@ -1115,11 +1096,11 @@
         <v>44051</v>
       </c>
       <c r="C39" s="9" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D39" s="9"/>
       <c r="E39" s="11" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F39" s="10"/>
       <c r="G39" s="11"/>
@@ -1133,11 +1114,11 @@
         <v>44100</v>
       </c>
       <c r="C40" s="9" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D40" s="9"/>
       <c r="E40" s="11" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F40" s="10"/>
       <c r="G40" s="11"/>
@@ -1152,11 +1133,11 @@
         <v>44135</v>
       </c>
       <c r="C41" s="9" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D41" s="9"/>
       <c r="E41" s="11" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F41" s="10"/>
       <c r="H41" s="11"/>
@@ -1186,11 +1167,11 @@
         <v>44156</v>
       </c>
       <c r="C43" s="9" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D43" s="9"/>
       <c r="E43" s="11" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F43" s="10"/>
       <c r="H43" s="11"/>
@@ -1203,11 +1184,11 @@
         <v>44177</v>
       </c>
       <c r="C44" s="9" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D44" s="9"/>
       <c r="E44" s="11" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F44" s="10"/>
       <c r="H44" s="11"/>
@@ -1224,7 +1205,7 @@
       </c>
       <c r="D45" s="9"/>
       <c r="E45" s="11" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="F45" s="10"/>
       <c r="H45" s="11"/>
@@ -1241,7 +1222,7 @@
       </c>
       <c r="D46" s="9"/>
       <c r="E46" s="11" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F46" s="10"/>
       <c r="H46" s="11"/>
@@ -1254,7 +1235,7 @@
         <v>44226</v>
       </c>
       <c r="C47" s="9" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D47" s="9"/>
       <c r="E47" s="11" t="s">
@@ -1271,7 +1252,7 @@
         <v>44240</v>
       </c>
       <c r="C48" s="9" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D48" s="9"/>
       <c r="E48" s="11" t="s">
@@ -1292,7 +1273,7 @@
       </c>
       <c r="D49" s="9"/>
       <c r="E49" s="11" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F49" s="10"/>
       <c r="H49" s="11"/>
@@ -1305,11 +1286,11 @@
         <v>44268</v>
       </c>
       <c r="C50" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D50" s="9"/>
       <c r="E50" s="11" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F50" s="10"/>
       <c r="H50" s="11"/>
@@ -1322,11 +1303,11 @@
         <v>44296</v>
       </c>
       <c r="C51" s="11" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D51" s="11"/>
       <c r="E51" s="11" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F51" s="10"/>
       <c r="H51" s="11"/>
@@ -1340,11 +1321,11 @@
         <v>44317</v>
       </c>
       <c r="C52" s="11" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D52" s="11"/>
       <c r="E52" s="11" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F52" s="10"/>
       <c r="H52" s="11"/>
@@ -1357,11 +1338,11 @@
         <v>44331</v>
       </c>
       <c r="C53" s="11" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D53" s="11"/>
       <c r="E53" s="11" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F53" s="10"/>
       <c r="H53" s="11"/>
@@ -1374,11 +1355,11 @@
         <v>44345</v>
       </c>
       <c r="C54" s="11" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D54" s="11"/>
       <c r="E54" s="11" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F54" s="10"/>
       <c r="H54" s="11"/>
@@ -1395,7 +1376,7 @@
       </c>
       <c r="D55" s="11"/>
       <c r="E55" s="11" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F55" s="10"/>
       <c r="H55" s="11"/>
@@ -1412,7 +1393,7 @@
       </c>
       <c r="D56" s="9"/>
       <c r="E56" s="11" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F56" s="10"/>
       <c r="H56" s="11"/>
@@ -1425,11 +1406,11 @@
         <v>44408</v>
       </c>
       <c r="C57" s="11" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D57" s="11"/>
       <c r="E57" s="11" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F57" s="10"/>
       <c r="H57" s="11"/>
@@ -6163,7 +6144,6 @@
     <oddHeader/>
     <oddFooter/>
   </headerFooter>
-  <drawing r:id="rId2"/>
-  <legacyDrawing r:id="rId3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>